<commit_message>
fix summary script for new ver
</commit_message>
<xml_diff>
--- a/data/controls/github.xlsx
+++ b/data/controls/github.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\keaton\projects\recombinant-can\data\controls\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\drives.cscscience.ca\W\Projects\covid-19\analysis\ncov-recombinant\data\controls_representative\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18192" windowHeight="8508"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14748" windowHeight="6168"/>
   </bookViews>
   <sheets>
     <sheet name="github" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="132">
   <si>
     <t>gisaid_epi_isl</t>
   </si>
@@ -409,6 +409,12 @@
   </si>
   <si>
     <t>EPI_ISL_10714519</t>
+  </si>
+  <si>
+    <t>pango_lineage</t>
+  </si>
+  <si>
+    <t>XJ</t>
   </si>
 </sst>
 </file>
@@ -450,7 +456,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -513,11 +519,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFC6C6C6"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFC6C6C6"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -583,6 +602,9 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -888,891 +910,935 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.21875" style="5" customWidth="1"/>
-    <col min="2" max="2" width="16.5546875" style="6" customWidth="1"/>
-    <col min="3" max="4" width="20.44140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.88671875" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" style="7" customWidth="1"/>
-    <col min="9" max="9" width="43.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="47.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.21875" style="5" customWidth="1"/>
+    <col min="3" max="4" width="22.109375" style="6" customWidth="1"/>
+    <col min="5" max="6" width="20.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="21.88671875" style="7" customWidth="1"/>
+    <col min="10" max="10" width="43.5546875" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="C1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="31" t="s">
+        <v>130</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="22" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="C2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="D2" s="20"/>
+      <c r="E2" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="F2" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="19" t="s">
+      <c r="G2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="19" t="s">
+      <c r="H2" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="H2" s="21" t="s">
+      <c r="I2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="19" t="s">
+      <c r="J2" s="19" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="26" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="26" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="23" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="C3" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="D3" s="24"/>
+      <c r="E3" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="F3" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="23" t="s">
+      <c r="G3" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="H3" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="I3" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="J3" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="26" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" s="26" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="23" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="C4" s="24" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="25" t="s">
+      <c r="D4" s="24"/>
+      <c r="E4" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="F4" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="E4" s="23" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" s="23" t="s">
+      <c r="G4" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G4" s="23" t="s">
+      <c r="H4" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="H4" s="25" t="s">
+      <c r="I4" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="I4" s="23" t="s">
+      <c r="J4" s="23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="30" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" s="30" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="28" t="s">
+      <c r="C5" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="D5" s="28"/>
+      <c r="E5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="29" t="s">
+      <c r="F5" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="27" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="27" t="s">
+      <c r="G5" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="H5" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="29" t="s">
+      <c r="I5" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="I5" s="27" t="s">
+      <c r="J5" s="27" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="C6" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="D6" s="11"/>
+      <c r="E6" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="F6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="G6" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I6" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="C7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="8"/>
+      <c r="E7" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="F7" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="J7" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="C8" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="D8" s="8"/>
+      <c r="E8" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="F8" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G8" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I8" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="C9" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="4" t="s">
+      <c r="D9" s="8"/>
+      <c r="E9" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="F9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G9" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H9" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="J9" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="8"/>
+      <c r="E10" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="F10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="J10" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="C11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="15"/>
+      <c r="E11" s="16" t="s">
         <v>32</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="E11" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="G11" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H11" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I11" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="14" t="s">
+      <c r="J11" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="C12" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="D12" s="11"/>
+      <c r="E12" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="F12" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" s="10" t="s">
-        <v>58</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="G12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="12" t="s">
         <v>59</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="J12" s="10" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B13" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="8"/>
+      <c r="E13" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="F13" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" s="3" t="s">
+      <c r="G13" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G13" s="3" t="s">
+      <c r="H13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="I13" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="8" t="s">
+      <c r="C14" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="D14" s="8"/>
+      <c r="E14" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="F14" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F14" s="3" t="s">
+      <c r="G14" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G14" s="3" t="s">
+      <c r="H14" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="I14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="I14" s="3" t="s">
+      <c r="J14" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B15" s="8" t="s">
+      <c r="C15" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="C15" s="4" t="s">
+      <c r="D15" s="8"/>
+      <c r="E15" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="F15" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="3" t="s">
+      <c r="G15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="H15" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="I15" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="J15" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" s="17" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="B16" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="C16" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="D16" s="15"/>
+      <c r="E16" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="D16" s="16" t="s">
+      <c r="F16" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" s="14" t="s">
+      <c r="G16" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="H16" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="H16" s="16" t="s">
+      <c r="I16" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="I16" s="14" t="s">
+      <c r="J16" s="14" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:10" s="13" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>75</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="C17" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="D17" s="11"/>
+      <c r="E17" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="F17" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E17" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>34</v>
-      </c>
       <c r="G17" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="I17" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="I17" s="10" t="s">
+      <c r="J17" s="10" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B18" s="8" t="s">
+      <c r="C18" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="D18" s="8"/>
+      <c r="E18" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="F18" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G18" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="I18" s="3" t="s">
+      <c r="J18" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:10" s="9" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="C19" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="C19" s="4" t="s">
+      <c r="D19" s="8"/>
+      <c r="E19" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="F19" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G19" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="J19" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="C20" s="8" t="s">
         <v>89</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="D20" s="8"/>
+      <c r="E20" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="F20" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H20" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="J20" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="B21" s="8" t="s">
+      <c r="C21" s="8" t="s">
         <v>92</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="D21" s="8"/>
+      <c r="E21" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="F21" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G21" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H21" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I21" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="J21" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B22" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B22" s="8" t="s">
+      <c r="C22" s="8" t="s">
         <v>95</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="8"/>
+      <c r="E22" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="F22" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G22" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I22" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="J22" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B23" s="8" t="s">
+      <c r="C23" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="D23" s="8"/>
+      <c r="E23" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="F23" s="4" t="s">
         <v>78</v>
       </c>
-      <c r="E23" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G23" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H23" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H23" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I23" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="J23" s="3" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="17" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" s="17" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B24" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="C24" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C24" s="16" t="s">
+      <c r="D24" s="15"/>
+      <c r="E24" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="F24" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="E24" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="F24" s="14" t="s">
-        <v>34</v>
-      </c>
       <c r="G24" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="H24" s="29" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="I24" s="14" t="s">
+      <c r="J24" s="14" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="B25" s="8" t="s">
+      <c r="C25" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="D25" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="F25" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G25" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I25" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="J25" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="B26" s="8" t="s">
+      <c r="C26" s="8" t="s">
         <v>108</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="F26" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G26" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H26" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I26" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="J26" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B27" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="B27" s="8" t="s">
+      <c r="C27" s="8" t="s">
         <v>112</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="D27" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="F27" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F27" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G27" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I27" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="J27" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="B28" s="8" t="s">
+      <c r="C28" s="8" t="s">
         <v>114</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="D28" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="F28" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E28" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="F28" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G28" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H28" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I28" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="J28" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="B29" s="8" t="s">
+      <c r="C29" s="8" t="s">
         <v>117</v>
       </c>
-      <c r="C29" s="4" t="s">
+      <c r="D29" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="F29" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F29" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G29" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H29" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H29" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I29" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="J29" s="3" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" s="9" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B30" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="B30" s="8" t="s">
+      <c r="C30" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="D30" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="F30" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E30" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="F30" s="3" t="s">
-        <v>34</v>
-      </c>
       <c r="G30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H30" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I30" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="J30" s="3" t="s">
         <v>123</v>
       </c>
     </row>

</xml_diff>